<commit_message>
Extent report Integration Continued
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/LoginData.xlsx
+++ b/src/test/resources/Data/LoginData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Username</t>
   </si>
@@ -42,6 +42,15 @@
   </si>
   <si>
     <t>Admin</t>
+  </si>
+  <si>
+    <t>yolo</t>
+  </si>
+  <si>
+    <t>rule</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -362,7 +371,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,18 +409,18 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>